<commit_message>
add export folder path & promotion price for WAT
</commit_message>
<xml_diff>
--- a/target.xlsx
+++ b/target.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24617"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{838B4EF6-EF2D-4A68-AF85-C822244F596A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8ADF9A70-11D8-420E-A7C7-64A991CB85A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAN product" sheetId="1" r:id="rId1"/>
+    <sheet name="WAT url" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>MAN ID</t>
   </si>
@@ -35,6 +36,15 @@
   </si>
   <si>
     <t>433243</t>
+  </si>
+  <si>
+    <t>WAT url</t>
+  </si>
+  <si>
+    <t>https://www.watsons.com.hk/%E8%AD%B7%E8%88%92%E5%AF%B6radiant%E6%97%A5%E7%94%A824cm-9%E7%89%87/p/BP_287456</t>
+  </si>
+  <si>
+    <t>https://www.watsons.com.hk/%E6%BB%8B%E6%BD%A4%E8%82%B2%E9%AB%AE%E7%B2%BE%E8%8F%AF%E7%B4%A0/p/BP_266919</t>
   </si>
 </sst>
 </file>
@@ -53,9 +63,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -74,33 +87,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,48 +399,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="201.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="201.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="201.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="201.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2">
+      <c r="G1" s="1">
         <v>44495</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="G2" s="1">
         <v>44495</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="B3" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56225A47-D66B-4F66-B487-3C862EFE73DC}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3BE67645-1947-4C4C-B9EF-F9B51F594E1A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{59C5E996-631A-403F-987A-7E03910BF5DF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more promotion mesage handler
</commit_message>
<xml_diff>
--- a/target.xlsx
+++ b/target.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25001633\Documents\daily record\ManningsPricing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171F0C86-48AA-4839-A268-1472DDDF6BA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D54777-11B9-4113-A484-2FE101B684B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1755" windowWidth="14400" windowHeight="14445" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAN product" sheetId="1" r:id="rId1"/>
@@ -1046,196 +1046,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56225A47-D66B-4F66-B487-3C862EFE73DC}">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="K2" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>53</v>
+      <c r="A20" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>55</v>
+      <c r="A21" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>58</v>
+      <c r="A22" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>60</v>
+      <c r="A23" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>91</v>
+      <c r="A24" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>92</v>
+      <c r="A27" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>100</v>
+      <c r="A34" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>101</v>
+      <c r="A35" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1247,21 +1245,22 @@
     <hyperlink ref="A7" r:id="rId4" xr:uid="{E603C767-6275-4250-AF90-B2E3DE41DE49}"/>
     <hyperlink ref="A9" r:id="rId5" xr:uid="{62571574-719E-4A79-B9A8-ACCD831EEB39}"/>
     <hyperlink ref="A10" r:id="rId6" xr:uid="{244538C0-B4F2-402A-9B8E-650CDBDCA719}"/>
-    <hyperlink ref="A17" r:id="rId7" xr:uid="{9DA80DA6-F0CC-4F26-A9D1-7B99BE6E2C46}"/>
-    <hyperlink ref="A16" r:id="rId8" xr:uid="{0256B479-E684-4949-9349-688B811EFA1D}"/>
-    <hyperlink ref="A19" r:id="rId9" xr:uid="{D6D17C8D-6E14-45D7-A47D-1D29BDE5F1C3}"/>
-    <hyperlink ref="A18" r:id="rId10" xr:uid="{42D381C5-EA2F-46B9-A9F5-28EBBCE33A59}"/>
-    <hyperlink ref="A27" r:id="rId11" xr:uid="{70AD2839-51E4-467D-8341-A95D2C2FF67B}"/>
-    <hyperlink ref="A26" r:id="rId12" xr:uid="{5CEB37DB-0F8D-4EDD-9468-6C1B409B5093}"/>
-    <hyperlink ref="A28" r:id="rId13" xr:uid="{FA4EAB9F-A74D-4979-B424-2218E2A357CD}"/>
-    <hyperlink ref="A29" r:id="rId14" xr:uid="{DA8FEB38-962E-4C3C-8859-D83C5D65A2B2}"/>
-    <hyperlink ref="A30" r:id="rId15" xr:uid="{61F02761-FED9-4F6F-BBFB-3DEC63745157}"/>
-    <hyperlink ref="A31" r:id="rId16" xr:uid="{B44B2E3B-C068-420D-973B-F5999106EA5C}"/>
-    <hyperlink ref="A32" r:id="rId17" xr:uid="{53D897B3-C0D6-4842-B1C2-08A8078098C1}"/>
-    <hyperlink ref="A33" r:id="rId18" xr:uid="{59E0CEBE-63BF-400D-BFF3-83C03D90531D}"/>
-    <hyperlink ref="A34" r:id="rId19" xr:uid="{878EB227-0000-416D-B300-805CB39DD93E}"/>
-    <hyperlink ref="A36" r:id="rId20" xr:uid="{16C8FC18-A8FA-41A7-85A1-C4D2ABADF2C9}"/>
-    <hyperlink ref="A37" r:id="rId21" xr:uid="{9602D3C3-8B9E-46D5-8C6E-5AB90B044B55}"/>
+    <hyperlink ref="A16" r:id="rId7" xr:uid="{9DA80DA6-F0CC-4F26-A9D1-7B99BE6E2C46}"/>
+    <hyperlink ref="A15" r:id="rId8" xr:uid="{0256B479-E684-4949-9349-688B811EFA1D}"/>
+    <hyperlink ref="A18" r:id="rId9" xr:uid="{D6D17C8D-6E14-45D7-A47D-1D29BDE5F1C3}"/>
+    <hyperlink ref="A17" r:id="rId10" xr:uid="{42D381C5-EA2F-46B9-A9F5-28EBBCE33A59}"/>
+    <hyperlink ref="A26" r:id="rId11" xr:uid="{70AD2839-51E4-467D-8341-A95D2C2FF67B}"/>
+    <hyperlink ref="A25" r:id="rId12" xr:uid="{5CEB37DB-0F8D-4EDD-9468-6C1B409B5093}"/>
+    <hyperlink ref="A27" r:id="rId13" xr:uid="{FA4EAB9F-A74D-4979-B424-2218E2A357CD}"/>
+    <hyperlink ref="A28" r:id="rId14" xr:uid="{DA8FEB38-962E-4C3C-8859-D83C5D65A2B2}"/>
+    <hyperlink ref="A29" r:id="rId15" xr:uid="{61F02761-FED9-4F6F-BBFB-3DEC63745157}"/>
+    <hyperlink ref="A30" r:id="rId16" xr:uid="{B44B2E3B-C068-420D-973B-F5999106EA5C}"/>
+    <hyperlink ref="A31" r:id="rId17" xr:uid="{53D897B3-C0D6-4842-B1C2-08A8078098C1}"/>
+    <hyperlink ref="A32" r:id="rId18" xr:uid="{59E0CEBE-63BF-400D-BFF3-83C03D90531D}"/>
+    <hyperlink ref="A33" r:id="rId19" xr:uid="{878EB227-0000-416D-B300-805CB39DD93E}"/>
+    <hyperlink ref="A35" r:id="rId20" xr:uid="{16C8FC18-A8FA-41A7-85A1-C4D2ABADF2C9}"/>
+    <hyperlink ref="A36" r:id="rId21" xr:uid="{9602D3C3-8B9E-46D5-8C6E-5AB90B044B55}"/>
+    <hyperlink ref="A11" r:id="rId22" xr:uid="{576230D7-7DF4-46DC-9AB7-DC0024E80571}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>